<commit_message>
added multiple objective ga optimization
</commit_message>
<xml_diff>
--- a/figs/snakes_dec17/PVE_active_contours.xlsx
+++ b/figs/snakes_dec17/PVE_active_contours.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="45">
   <si>
     <t xml:space="preserve">Edges</t>
   </si>
@@ -155,6 +156,9 @@
   <si>
     <t xml:space="preserve">Snakes – 2412-01</t>
   </si>
+  <si>
+    <t xml:space="preserve">Snakes – 040118</t>
+  </si>
 </sst>
 </file>
 
@@ -165,7 +169,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -205,6 +209,13 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFF3300"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF009900"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -252,7 +263,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -289,6 +300,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -309,7 +324,7 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF009900"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -369,7 +384,7 @@
   <dimension ref="A1:U46"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3103,8 +3118,8 @@
   </sheetPr>
   <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D54" activeCellId="0" sqref="D54"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4638,4 +4653,349 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.9897959183674"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>52295.681</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>25264.893</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>22822.453</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>25799.604</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>50882.94</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">AVERAGE(B2:F2)</f>
+        <v>35413.1142</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">MAX(B2:F2)</f>
+        <v>52295.681</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <f aca="false">MIN(B2:F2)</f>
+        <v>22822.453</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>47610.955</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>25605.469</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>21790.472</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>24998.141</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>47615.576</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">AVERAGE(B3:F3)</f>
+        <v>33524.1226</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">MAX(B3:F3)</f>
+        <v>47615.576</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">MIN(B3:F3)</f>
+        <v>21790.472</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>-0.013</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <f aca="false">AVERAGE(B4:F4)</f>
+        <v>0.0434</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <f aca="false">MAX(B4:F4)</f>
+        <v>0.09</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <f aca="false">MIN(B4:F4)</f>
+        <v>-0.013</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>32805.908</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>9591.064</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>11771.3</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>15589.534</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>34140.034</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">AVERAGE(B5:F5)</f>
+        <v>20779.568</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">MAX(B5:F5)</f>
+        <v>34140.034</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">MIN(B5:F5)</f>
+        <v>9591.064</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>28119.757</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>10344.238</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>10443.852</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>14772.479</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>34042.368</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">AVERAGE(B6:F6)</f>
+        <v>19544.5388</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">MAX(B6:F6)</f>
+        <v>34042.368</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <f aca="false">MIN(B6:F6)</f>
+        <v>10344.238</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>-0.079</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <f aca="false">AVERAGE(B7:F7)</f>
+        <v>0.0464</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <f aca="false">MAX(B7:F7)</f>
+        <v>0.143</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <f aca="false">MIN(B7:F7)</f>
+        <v>-0.079</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>19489.773</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>15673.828</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>11051.153</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>10210.069</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>16742.907</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">AVERAGE(B8:F8)</f>
+        <v>14633.546</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">MAX(B8:F8)</f>
+        <v>19489.773</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">MIN(B8:F8)</f>
+        <v>10210.069</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>19491.198</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>15261.23</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>11346.62</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>10225.662</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>13573.208</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">AVERAGE(B9:F9)</f>
+        <v>13979.5836</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <f aca="false">MAX(B9:F9)</f>
+        <v>19491.198</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <f aca="false">MIN(B9:F9)</f>
+        <v>10225.662</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>-0.027</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>-0.002</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>0.189</v>
+      </c>
+      <c r="G10" s="9" t="n">
+        <f aca="false">AVERAGE(B10:F10)</f>
+        <v>0.0372</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <f aca="false">MAX(B10:F10)</f>
+        <v>0.189</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <f aca="false">MIN(B10:F10)</f>
+        <v>-0.027</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>